<commit_message>
refactor: clean up for openpyxl-only engine and add example usage
</commit_message>
<xml_diff>
--- a/tests/data/sample.xlsx
+++ b/tests/data/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ychoe\Downloads\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ychoe\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2F7045-13D8-4BC7-A56F-38E91BE5CBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF9CEEE-FB0B-4AFC-A13F-F29E72FE029D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="18700" xr2:uid="{383B7338-DE7F-4A6B-AF2C-22EC87D8D257}"/>
   </bookViews>
@@ -36,18 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Alice</t>
   </si>
   <si>
     <t>Bob</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Eve</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -435,20 +438,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91035E99-D78F-4561-8DD2-2E8F53FC59C5}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -456,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,6 +467,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add WHERE condition support for SELECT queries
docs: add detailed docstrings for OpenpyxlEngine and OpenpyxlExecutor
</commit_message>
<xml_diff>
--- a/tests/data/sample.xlsx
+++ b/tests/data/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ychoe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeongseonchoe/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF9CEEE-FB0B-4AFC-A13F-F29E72FE029D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D597056-6253-4342-82E0-6C7C285B335C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="18700" xr2:uid="{383B7338-DE7F-4A6B-AF2C-22EC87D8D257}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="29020" windowHeight="18700" xr2:uid="{383B7338-DE7F-4A6B-AF2C-22EC87D8D257}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,13 +44,13 @@
     <t>Bob</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Eve</t>
   </si>
   <si>
-    <t>Id</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -441,20 +441,20 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -462,7 +462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -470,12 +470,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>